<commit_message>
updates value ranges in trap and release metadata tables
</commit_message>
<xml_diff>
--- a/data-raw/metadata/camp_release_metadata.xlsx
+++ b/data-raw/metadata/camp_release_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleyvizek/code/jpe-knights-edi/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A365C77-3B88-AB4C-BDF9-D536455A2CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E3D5C0-4E04-F24F-B870-D62B2BF45C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="68640" yWindow="-12120" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="317">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -191,9 +191,6 @@
   </si>
   <si>
     <t>Number of days this trap test is considered valid</t>
-  </si>
-  <si>
-    <t>days</t>
   </si>
   <si>
     <t>includeTestID</t>
@@ -969,6 +966,18 @@
   <si>
     <t>sourceOfFishSiteID</t>
   </si>
+  <si>
+    <t>count of fish</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>2006-12-18 05:15:50</t>
+  </si>
+  <si>
+    <t>2022-04-15 02:45:20</t>
+  </si>
 </sst>
 </file>
 
@@ -1043,7 +1052,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1083,6 +1092,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1300,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1643,7 +1655,7 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>33</v>
@@ -1774,15 +1786,21 @@
       <c r="F12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>313</v>
+      </c>
       <c r="H12" s="3" t="s">
         <v>42</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
+        <v>407</v>
+      </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -1816,15 +1834,21 @@
       <c r="F13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>313</v>
+      </c>
       <c r="H13" s="3" t="s">
         <v>42</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="3"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
+      <c r="L13" s="3">
+        <v>0</v>
+      </c>
+      <c r="M13" s="3">
+        <v>46</v>
+      </c>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1858,15 +1882,21 @@
       <c r="F14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>313</v>
+      </c>
       <c r="H14" s="3" t="s">
         <v>42</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="L14" s="3">
+        <v>81</v>
+      </c>
+      <c r="M14" s="3">
+        <v>7180</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1905,8 +1935,12 @@
         <v>50</v>
       </c>
       <c r="K15" s="2"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="L15" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="M15" s="19" t="s">
+        <v>316</v>
+      </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1979,7 +2013,7 @@
         <v>40</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>55</v>
+        <v>314</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>42</v>
@@ -1987,8 +2021,12 @@
       <c r="I17" s="2"/>
       <c r="J17" s="3"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
+      <c r="L17" s="3">
+        <v>0</v>
+      </c>
+      <c r="M17" s="3">
+        <v>136</v>
+      </c>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -2005,10 +2043,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
@@ -2043,10 +2081,10 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
@@ -2081,10 +2119,10 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>15</v>
@@ -2119,10 +2157,10 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>15</v>
@@ -2157,10 +2195,10 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>15</v>
@@ -29785,13 +29823,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
@@ -29822,7 +29860,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>13</v>
@@ -29856,7 +29894,7 @@
         <v>159697</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>24</v>
@@ -29890,7 +29928,7 @@
         <v>159698</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>24</v>
@@ -29924,7 +29962,7 @@
         <v>159700</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>24</v>
@@ -29958,7 +29996,7 @@
         <v>159707</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>24</v>
@@ -29992,7 +30030,7 @@
         <v>159709</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>24</v>
@@ -30026,7 +30064,7 @@
         <v>159710</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>24</v>
@@ -30060,7 +30098,7 @@
         <v>159713</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>24</v>
@@ -30094,7 +30132,7 @@
         <v>161030</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>24</v>
@@ -30128,7 +30166,7 @@
         <v>161064</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>24</v>
@@ -30162,7 +30200,7 @@
         <v>161067</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>24</v>
@@ -30196,7 +30234,7 @@
         <v>161068</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>24</v>
@@ -30230,7 +30268,7 @@
         <v>161127</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>24</v>
@@ -30264,7 +30302,7 @@
         <v>161702</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>24</v>
@@ -30298,7 +30336,7 @@
         <v>161738</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>24</v>
@@ -30332,7 +30370,7 @@
         <v>161931</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>24</v>
@@ -30366,7 +30404,7 @@
         <v>161974</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>24</v>
@@ -30400,7 +30438,7 @@
         <v>161975</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>24</v>
@@ -30434,7 +30472,7 @@
         <v>161977</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>24</v>
@@ -30468,7 +30506,7 @@
         <v>161979</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>24</v>
@@ -30502,7 +30540,7 @@
         <v>161980</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>24</v>
@@ -30536,7 +30574,7 @@
         <v>161989</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>24</v>
@@ -30570,7 +30608,7 @@
         <v>161997</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>24</v>
@@ -30604,7 +30642,7 @@
         <v>162003</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>24</v>
@@ -30638,7 +30676,7 @@
         <v>162032</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>24</v>
@@ -30672,7 +30710,7 @@
         <v>162033</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>24</v>
@@ -30706,7 +30744,7 @@
         <v>163342</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>24</v>
@@ -30740,7 +30778,7 @@
         <v>163344</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>24</v>
@@ -30774,7 +30812,7 @@
         <v>163350</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>24</v>
@@ -30808,7 +30846,7 @@
         <v>163368</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>24</v>
@@ -30842,7 +30880,7 @@
         <v>163387</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>24</v>
@@ -30876,7 +30914,7 @@
         <v>163517</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>24</v>
@@ -30910,7 +30948,7 @@
         <v>163524</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>24</v>
@@ -30944,7 +30982,7 @@
         <v>163565</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>24</v>
@@ -30978,7 +31016,7 @@
         <v>163569</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>24</v>
@@ -31012,7 +31050,7 @@
         <v>163587</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>24</v>
@@ -31046,7 +31084,7 @@
         <v>163589</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>24</v>
@@ -31080,7 +31118,7 @@
         <v>163603</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>24</v>
@@ -31114,7 +31152,7 @@
         <v>163792</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>24</v>
@@ -31148,7 +31186,7 @@
         <v>163892</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>24</v>
@@ -31182,7 +31220,7 @@
         <v>163908</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>24</v>
@@ -31216,7 +31254,7 @@
         <v>163995</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>24</v>
@@ -31250,7 +31288,7 @@
         <v>163998</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>24</v>
@@ -31284,7 +31322,7 @@
         <v>164034</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>24</v>
@@ -31318,7 +31356,7 @@
         <v>164037</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>24</v>
@@ -31352,7 +31390,7 @@
         <v>164039</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>24</v>
@@ -31386,7 +31424,7 @@
         <v>164041</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>24</v>
@@ -31420,7 +31458,7 @@
         <v>164043</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C49" s="14" t="s">
         <v>24</v>
@@ -31454,7 +31492,7 @@
         <v>165679</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C50" s="14" t="s">
         <v>24</v>
@@ -31488,7 +31526,7 @@
         <v>165877</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C51" s="14" t="s">
         <v>24</v>
@@ -31522,7 +31560,7 @@
         <v>165878</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C52" s="14" t="s">
         <v>24</v>
@@ -31556,7 +31594,7 @@
         <v>165993</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C53" s="14" t="s">
         <v>24</v>
@@ -31590,7 +31628,7 @@
         <v>165998</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C54" s="14" t="s">
         <v>24</v>
@@ -31624,7 +31662,7 @@
         <v>166365</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C55" s="14" t="s">
         <v>24</v>
@@ -31658,7 +31696,7 @@
         <v>167229</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C56" s="14" t="s">
         <v>24</v>
@@ -31692,7 +31730,7 @@
         <v>167233</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C57" s="14" t="s">
         <v>24</v>
@@ -31726,7 +31764,7 @@
         <v>167234</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C58" s="14" t="s">
         <v>24</v>
@@ -31760,7 +31798,7 @@
         <v>167680</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C59" s="14" t="s">
         <v>24</v>
@@ -31794,7 +31832,7 @@
         <v>168093</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>24</v>
@@ -31828,7 +31866,7 @@
         <v>168130</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>24</v>
@@ -31862,7 +31900,7 @@
         <v>168132</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>24</v>
@@ -31896,7 +31934,7 @@
         <v>168139</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C63" s="14" t="s">
         <v>24</v>
@@ -31930,7 +31968,7 @@
         <v>168141</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C64" s="14" t="s">
         <v>24</v>
@@ -31964,7 +32002,7 @@
         <v>168144</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C65" s="14" t="s">
         <v>24</v>
@@ -31998,7 +32036,7 @@
         <v>168154</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C66" s="14" t="s">
         <v>24</v>
@@ -32032,7 +32070,7 @@
         <v>168158</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C67" s="14" t="s">
         <v>24</v>
@@ -32066,7 +32104,7 @@
         <v>168160</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C68" s="14" t="s">
         <v>24</v>
@@ -32100,7 +32138,7 @@
         <v>168161</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C69" s="14" t="s">
         <v>24</v>
@@ -32134,7 +32172,7 @@
         <v>168163</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C70" s="14" t="s">
         <v>24</v>
@@ -32168,7 +32206,7 @@
         <v>168165</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C71" s="14" t="s">
         <v>24</v>
@@ -32202,7 +32240,7 @@
         <v>168166</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C72" s="14" t="s">
         <v>24</v>
@@ -32236,7 +32274,7 @@
         <v>168167</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>24</v>
@@ -32270,7 +32308,7 @@
         <v>168175</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C74" s="14" t="s">
         <v>24</v>
@@ -32304,7 +32342,7 @@
         <v>168487</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>24</v>
@@ -32338,7 +32376,7 @@
         <v>171882</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C76" s="14" t="s">
         <v>24</v>
@@ -32372,7 +32410,7 @@
         <v>250</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C77" s="14" t="s">
         <v>24</v>
@@ -32406,7 +32444,7 @@
         <v>251</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C78" s="14" t="s">
         <v>24</v>
@@ -32440,7 +32478,7 @@
         <v>252</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C79" s="14" t="s">
         <v>24</v>
@@ -32474,7 +32512,7 @@
         <v>253</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C80" s="14" t="s">
         <v>24</v>
@@ -32508,7 +32546,7 @@
         <v>254</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C81" s="14" t="s">
         <v>24</v>
@@ -32542,7 +32580,7 @@
         <v>255</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C82" s="14" t="s">
         <v>24</v>
@@ -32576,7 +32614,7 @@
         <v>550562</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C83" s="14" t="s">
         <v>24</v>
@@ -32610,7 +32648,7 @@
         <v>553322</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C84" s="14" t="s">
         <v>24</v>
@@ -32644,7 +32682,7 @@
         <v>622248</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C85" s="14" t="s">
         <v>24</v>
@@ -32678,7 +32716,7 @@
         <v>3</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C86" s="14" t="s">
         <v>26</v>
@@ -32712,7 +32750,7 @@
         <v>5</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C87" s="14" t="s">
         <v>26</v>
@@ -32746,7 +32784,7 @@
         <v>6</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C88" s="14" t="s">
         <v>26</v>
@@ -32780,7 +32818,7 @@
         <v>252</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C89" s="14" t="s">
         <v>26</v>
@@ -32814,7 +32852,7 @@
         <v>251</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C90" s="14" t="s">
         <v>26</v>
@@ -32848,7 +32886,7 @@
         <v>255</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C91" s="14" t="s">
         <v>26</v>
@@ -32882,7 +32920,7 @@
         <v>250</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C92" s="14" t="s">
         <v>26</v>
@@ -32916,7 +32954,7 @@
         <v>254</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C93" s="14" t="s">
         <v>26</v>
@@ -32950,7 +32988,7 @@
         <v>1</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C94" s="14" t="s">
         <v>26</v>
@@ -32984,7 +33022,7 @@
         <v>2</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C95" s="14" t="s">
         <v>26</v>
@@ -33018,7 +33056,7 @@
         <v>253</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C96" s="14" t="s">
         <v>26</v>
@@ -33052,7 +33090,7 @@
         <v>4</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C97" s="14" t="s">
         <v>26</v>
@@ -33086,7 +33124,7 @@
         <v>11</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C98" s="14" t="s">
         <v>28</v>
@@ -33120,7 +33158,7 @@
         <v>6</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C99" s="14" t="s">
         <v>28</v>
@@ -33154,7 +33192,7 @@
         <v>12</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C100" s="14" t="s">
         <v>28</v>
@@ -33188,7 +33226,7 @@
         <v>17</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C101" s="14" t="s">
         <v>28</v>
@@ -33222,7 +33260,7 @@
         <v>3</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C102" s="14" t="s">
         <v>28</v>
@@ -33256,7 +33294,7 @@
         <v>15</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C103" s="14" t="s">
         <v>28</v>
@@ -33290,7 +33328,7 @@
         <v>10</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C104" s="14" t="s">
         <v>28</v>
@@ -33324,7 +33362,7 @@
         <v>16</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C105" s="14" t="s">
         <v>28</v>
@@ -33358,7 +33396,7 @@
         <v>13</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C106" s="14" t="s">
         <v>28</v>
@@ -33392,7 +33430,7 @@
         <v>14</v>
       </c>
       <c r="B107" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C107" s="14" t="s">
         <v>28</v>
@@ -33426,7 +33464,7 @@
         <v>252</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C108" s="14" t="s">
         <v>28</v>
@@ -33460,7 +33498,7 @@
         <v>251</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C109" s="14" t="s">
         <v>28</v>
@@ -33494,7 +33532,7 @@
         <v>255</v>
       </c>
       <c r="B110" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C110" s="14" t="s">
         <v>28</v>
@@ -33528,7 +33566,7 @@
         <v>250</v>
       </c>
       <c r="B111" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C111" s="14" t="s">
         <v>28</v>
@@ -33562,7 +33600,7 @@
         <v>4</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C112" s="14" t="s">
         <v>28</v>
@@ -33596,7 +33634,7 @@
         <v>7</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C113" s="14" t="s">
         <v>28</v>
@@ -33630,7 +33668,7 @@
         <v>19</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C114" s="14" t="s">
         <v>28</v>
@@ -33664,7 +33702,7 @@
         <v>254</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C115" s="14" t="s">
         <v>28</v>
@@ -33698,7 +33736,7 @@
         <v>5</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C116" s="14" t="s">
         <v>28</v>
@@ -33732,7 +33770,7 @@
         <v>8</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C117" s="14" t="s">
         <v>28</v>
@@ -33766,7 +33804,7 @@
         <v>20</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C118" s="14" t="s">
         <v>28</v>
@@ -33800,7 +33838,7 @@
         <v>18</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C119" s="14" t="s">
         <v>28</v>
@@ -33834,7 +33872,7 @@
         <v>253</v>
       </c>
       <c r="B120" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C120" s="14" t="s">
         <v>28</v>
@@ -33868,7 +33906,7 @@
         <v>9</v>
       </c>
       <c r="B121" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C121" s="14" t="s">
         <v>28</v>
@@ -33902,7 +33940,7 @@
         <v>1</v>
       </c>
       <c r="B122" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C122" s="14" t="s">
         <v>28</v>
@@ -33936,7 +33974,7 @@
         <v>2</v>
       </c>
       <c r="B123" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C123" s="14" t="s">
         <v>28</v>
@@ -33970,7 +34008,7 @@
         <v>1</v>
       </c>
       <c r="B124" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C124" s="14" t="s">
         <v>30</v>
@@ -34004,7 +34042,7 @@
         <v>3</v>
       </c>
       <c r="B125" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C125" s="14" t="s">
         <v>30</v>
@@ -34038,7 +34076,7 @@
         <v>2</v>
       </c>
       <c r="B126" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C126" s="14" t="s">
         <v>30</v>
@@ -34072,7 +34110,7 @@
         <v>252</v>
       </c>
       <c r="B127" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C127" s="14" t="s">
         <v>30</v>
@@ -34106,7 +34144,7 @@
         <v>251</v>
       </c>
       <c r="B128" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C128" s="14" t="s">
         <v>30</v>
@@ -34140,7 +34178,7 @@
         <v>255</v>
       </c>
       <c r="B129" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C129" s="14" t="s">
         <v>30</v>
@@ -34174,7 +34212,7 @@
         <v>250</v>
       </c>
       <c r="B130" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C130" s="14" t="s">
         <v>30</v>
@@ -34208,7 +34246,7 @@
         <v>254</v>
       </c>
       <c r="B131" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C131" s="14" t="s">
         <v>30</v>
@@ -34242,7 +34280,7 @@
         <v>253</v>
       </c>
       <c r="B132" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C132" s="14" t="s">
         <v>30</v>
@@ -34276,7 +34314,7 @@
         <v>3000</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C133" s="14" t="s">
         <v>32</v>
@@ -34310,7 +34348,7 @@
         <v>44000</v>
       </c>
       <c r="B134" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C134" s="14" t="s">
         <v>32</v>
@@ -34344,7 +34382,7 @@
         <v>52000</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C135" s="14" t="s">
         <v>32</v>
@@ -34378,7 +34416,7 @@
         <v>51000</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C136" s="14" t="s">
         <v>32</v>
@@ -34412,7 +34450,7 @@
         <v>5000</v>
       </c>
       <c r="B137" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C137" s="14" t="s">
         <v>32</v>
@@ -34446,7 +34484,7 @@
         <v>46000</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C138" s="14" t="s">
         <v>32</v>
@@ -34480,7 +34518,7 @@
         <v>4000</v>
       </c>
       <c r="B139" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C139" s="14" t="s">
         <v>32</v>
@@ -34514,7 +34552,7 @@
         <v>45000</v>
       </c>
       <c r="B140" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C140" s="14" t="s">
         <v>32</v>
@@ -34548,7 +34586,7 @@
         <v>252</v>
       </c>
       <c r="B141" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C141" s="14" t="s">
         <v>32</v>
@@ -34582,7 +34620,7 @@
         <v>251</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C142" s="14" t="s">
         <v>32</v>
@@ -34616,7 +34654,7 @@
         <v>255</v>
       </c>
       <c r="B143" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C143" s="14" t="s">
         <v>32</v>
@@ -34650,7 +34688,7 @@
         <v>53000</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C144" s="14" t="s">
         <v>32</v>
@@ -34684,7 +34722,7 @@
         <v>54000</v>
       </c>
       <c r="B145" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C145" s="14" t="s">
         <v>32</v>
@@ -34718,7 +34756,7 @@
         <v>55000</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C146" s="14" t="s">
         <v>32</v>
@@ -34752,7 +34790,7 @@
         <v>56000</v>
       </c>
       <c r="B147" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C147" s="14" t="s">
         <v>32</v>
@@ -34786,7 +34824,7 @@
         <v>50000</v>
       </c>
       <c r="B148" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C148" s="14" t="s">
         <v>32</v>
@@ -34820,7 +34858,7 @@
         <v>7000</v>
       </c>
       <c r="B149" s="13" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C149" s="14" t="s">
         <v>32</v>
@@ -34854,7 +34892,7 @@
         <v>2000</v>
       </c>
       <c r="B150" s="13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C150" s="14" t="s">
         <v>32</v>
@@ -34888,7 +34926,7 @@
         <v>43000</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C151" s="14" t="s">
         <v>32</v>
@@ -34922,7 +34960,7 @@
         <v>6000</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C152" s="14" t="s">
         <v>32</v>
@@ -34956,7 +34994,7 @@
         <v>47000</v>
       </c>
       <c r="B153" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C153" s="14" t="s">
         <v>32</v>
@@ -34990,7 +35028,7 @@
         <v>90000</v>
       </c>
       <c r="B154" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C154" s="14" t="s">
         <v>32</v>
@@ -35024,7 +35062,7 @@
         <v>253</v>
       </c>
       <c r="B155" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C155" s="14" t="s">
         <v>32</v>
@@ -35058,7 +35096,7 @@
         <v>3000</v>
       </c>
       <c r="B156" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C156" s="14" t="s">
         <v>34</v>
@@ -35092,7 +35130,7 @@
         <v>44000</v>
       </c>
       <c r="B157" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C157" s="14" t="s">
         <v>34</v>
@@ -35126,7 +35164,7 @@
         <v>52000</v>
       </c>
       <c r="B158" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C158" s="14" t="s">
         <v>34</v>
@@ -35160,7 +35198,7 @@
         <v>51000</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C159" s="14" t="s">
         <v>34</v>
@@ -35194,7 +35232,7 @@
         <v>5000</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C160" s="14" t="s">
         <v>34</v>
@@ -35228,7 +35266,7 @@
         <v>46000</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C161" s="14" t="s">
         <v>34</v>
@@ -35262,7 +35300,7 @@
         <v>4000</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C162" s="14" t="s">
         <v>34</v>
@@ -35296,7 +35334,7 @@
         <v>45000</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C163" s="14" t="s">
         <v>34</v>
@@ -35330,7 +35368,7 @@
         <v>252</v>
       </c>
       <c r="B164" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C164" s="14" t="s">
         <v>34</v>
@@ -35364,7 +35402,7 @@
         <v>251</v>
       </c>
       <c r="B165" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C165" s="14" t="s">
         <v>34</v>
@@ -35398,7 +35436,7 @@
         <v>255</v>
       </c>
       <c r="B166" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C166" s="14" t="s">
         <v>34</v>
@@ -35432,7 +35470,7 @@
         <v>53000</v>
       </c>
       <c r="B167" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C167" s="14" t="s">
         <v>34</v>
@@ -35466,7 +35504,7 @@
         <v>54000</v>
       </c>
       <c r="B168" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C168" s="14" t="s">
         <v>34</v>
@@ -35500,7 +35538,7 @@
         <v>55000</v>
       </c>
       <c r="B169" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C169" s="14" t="s">
         <v>34</v>
@@ -35534,7 +35572,7 @@
         <v>56000</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C170" s="14" t="s">
         <v>34</v>
@@ -35568,7 +35606,7 @@
         <v>50000</v>
       </c>
       <c r="B171" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C171" s="14" t="s">
         <v>34</v>
@@ -35602,7 +35640,7 @@
         <v>7000</v>
       </c>
       <c r="B172" s="13" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C172" s="14" t="s">
         <v>34</v>
@@ -35636,7 +35674,7 @@
         <v>2000</v>
       </c>
       <c r="B173" s="13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C173" s="14" t="s">
         <v>34</v>
@@ -35670,7 +35708,7 @@
         <v>43000</v>
       </c>
       <c r="B174" s="13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C174" s="14" t="s">
         <v>34</v>
@@ -35704,7 +35742,7 @@
         <v>6000</v>
       </c>
       <c r="B175" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C175" s="14" t="s">
         <v>34</v>
@@ -35738,7 +35776,7 @@
         <v>47000</v>
       </c>
       <c r="B176" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C176" s="14" t="s">
         <v>34</v>
@@ -35772,7 +35810,7 @@
         <v>90000</v>
       </c>
       <c r="B177" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C177" s="14" t="s">
         <v>34</v>
@@ -35806,7 +35844,7 @@
         <v>253</v>
       </c>
       <c r="B178" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C178" s="14" t="s">
         <v>34</v>
@@ -35840,7 +35878,7 @@
         <v>2001</v>
       </c>
       <c r="B179" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C179" s="14" t="s">
         <v>36</v>
@@ -35874,7 +35912,7 @@
         <v>44018</v>
       </c>
       <c r="B180" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C180" s="14" t="s">
         <v>36</v>
@@ -35908,7 +35946,7 @@
         <v>44007</v>
       </c>
       <c r="B181" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C181" s="14" t="s">
         <v>36</v>
@@ -35942,7 +35980,7 @@
         <v>44017</v>
       </c>
       <c r="B182" s="13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C182" s="14" t="s">
         <v>36</v>
@@ -35976,7 +36014,7 @@
         <v>44016</v>
       </c>
       <c r="B183" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C183" s="14" t="s">
         <v>36</v>
@@ -36010,7 +36048,7 @@
         <v>44013</v>
       </c>
       <c r="B184" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C184" s="14" t="s">
         <v>36</v>
@@ -36044,7 +36082,7 @@
         <v>3001</v>
       </c>
       <c r="B185" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C185" s="14" t="s">
         <v>36</v>
@@ -36078,7 +36116,7 @@
         <v>3002</v>
       </c>
       <c r="B186" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C186" s="14" t="s">
         <v>36</v>
@@ -36112,7 +36150,7 @@
         <v>52003</v>
       </c>
       <c r="B187" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C187" s="14" t="s">
         <v>36</v>
@@ -36146,7 +36184,7 @@
         <v>51002</v>
       </c>
       <c r="B188" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C188" s="14" t="s">
         <v>36</v>
@@ -36180,7 +36218,7 @@
         <v>51003</v>
       </c>
       <c r="B189" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C189" s="14" t="s">
         <v>36</v>
@@ -36214,7 +36252,7 @@
         <v>52001</v>
       </c>
       <c r="B190" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C190" s="14" t="s">
         <v>36</v>
@@ -36248,7 +36286,7 @@
         <v>52002</v>
       </c>
       <c r="B191" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C191" s="14" t="s">
         <v>36</v>
@@ -36282,7 +36320,7 @@
         <v>52004</v>
       </c>
       <c r="B192" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C192" s="14" t="s">
         <v>36</v>
@@ -36316,7 +36354,7 @@
         <v>90001</v>
       </c>
       <c r="B193" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C193" s="14" t="s">
         <v>36</v>
@@ -36350,7 +36388,7 @@
         <v>46003</v>
       </c>
       <c r="B194" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C194" s="14" t="s">
         <v>36</v>
@@ -36384,7 +36422,7 @@
         <v>46001</v>
       </c>
       <c r="B195" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C195" s="14" t="s">
         <v>36</v>
@@ -36418,7 +36456,7 @@
         <v>46004</v>
       </c>
       <c r="B196" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C196" s="14" t="s">
         <v>36</v>
@@ -36452,7 +36490,7 @@
         <v>5001</v>
       </c>
       <c r="B197" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C197" s="14" t="s">
         <v>36</v>
@@ -36486,7 +36524,7 @@
         <v>5003</v>
       </c>
       <c r="B198" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C198" s="14" t="s">
         <v>36</v>
@@ -36520,7 +36558,7 @@
         <v>5002</v>
       </c>
       <c r="B199" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C199" s="14" t="s">
         <v>36</v>
@@ -36554,7 +36592,7 @@
         <v>4001</v>
       </c>
       <c r="B200" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C200" s="14" t="s">
         <v>36</v>
@@ -36588,7 +36626,7 @@
         <v>4002</v>
       </c>
       <c r="B201" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C201" s="14" t="s">
         <v>36</v>
@@ -36622,7 +36660,7 @@
         <v>44010</v>
       </c>
       <c r="B202" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C202" s="14" t="s">
         <v>36</v>
@@ -36656,7 +36694,7 @@
         <v>51001</v>
       </c>
       <c r="B203" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C203" s="14" t="s">
         <v>36</v>
@@ -36690,7 +36728,7 @@
         <v>46002</v>
       </c>
       <c r="B204" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C204" s="14" t="s">
         <v>36</v>
@@ -36724,7 +36762,7 @@
         <v>43000</v>
       </c>
       <c r="B205" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C205" s="14" t="s">
         <v>36</v>
@@ -36758,7 +36796,7 @@
         <v>44000</v>
       </c>
       <c r="B206" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C206" s="14" t="s">
         <v>36</v>
@@ -36792,7 +36830,7 @@
         <v>45000</v>
       </c>
       <c r="B207" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C207" s="14" t="s">
         <v>36</v>
@@ -36826,7 +36864,7 @@
         <v>46000</v>
       </c>
       <c r="B208" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C208" s="14" t="s">
         <v>36</v>
@@ -36860,7 +36898,7 @@
         <v>47000</v>
       </c>
       <c r="B209" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C209" s="14" t="s">
         <v>36</v>
@@ -36894,7 +36932,7 @@
         <v>50000</v>
       </c>
       <c r="B210" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C210" s="14" t="s">
         <v>36</v>
@@ -36928,7 +36966,7 @@
         <v>51000</v>
       </c>
       <c r="B211" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C211" s="14" t="s">
         <v>36</v>
@@ -36962,7 +37000,7 @@
         <v>52000</v>
       </c>
       <c r="B212" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C212" s="14" t="s">
         <v>36</v>
@@ -36996,7 +37034,7 @@
         <v>53000</v>
       </c>
       <c r="B213" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C213" s="14" t="s">
         <v>36</v>
@@ -37030,7 +37068,7 @@
         <v>54000</v>
       </c>
       <c r="B214" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C214" s="14" t="s">
         <v>36</v>
@@ -37064,7 +37102,7 @@
         <v>55000</v>
       </c>
       <c r="B215" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C215" s="14" t="s">
         <v>36</v>
@@ -37098,7 +37136,7 @@
         <v>56000</v>
       </c>
       <c r="B216" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C216" s="14" t="s">
         <v>36</v>
@@ -37132,7 +37170,7 @@
         <v>90000</v>
       </c>
       <c r="B217" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C217" s="14" t="s">
         <v>36</v>
@@ -37166,7 +37204,7 @@
         <v>44001</v>
       </c>
       <c r="B218" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C218" s="14" t="s">
         <v>36</v>
@@ -37200,7 +37238,7 @@
         <v>44003</v>
       </c>
       <c r="B219" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C219" s="14" t="s">
         <v>36</v>
@@ -37234,7 +37272,7 @@
         <v>44002</v>
       </c>
       <c r="B220" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C220" s="14" t="s">
         <v>36</v>
@@ -37268,7 +37306,7 @@
         <v>44004</v>
       </c>
       <c r="B221" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C221" s="14" t="s">
         <v>36</v>
@@ -37302,7 +37340,7 @@
         <v>47002</v>
       </c>
       <c r="B222" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C222" s="14" t="s">
         <v>36</v>
@@ -37336,7 +37374,7 @@
         <v>47001</v>
       </c>
       <c r="B223" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C223" s="14" t="s">
         <v>36</v>
@@ -37370,7 +37408,7 @@
         <v>44009</v>
       </c>
       <c r="B224" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C224" s="14" t="s">
         <v>36</v>
@@ -37404,7 +37442,7 @@
         <v>44006</v>
       </c>
       <c r="B225" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C225" s="14" t="s">
         <v>36</v>
@@ -37438,7 +37476,7 @@
         <v>44008</v>
       </c>
       <c r="B226" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C226" s="14" t="s">
         <v>36</v>
@@ -37472,7 +37510,7 @@
         <v>7002</v>
       </c>
       <c r="B227" s="13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C227" s="14" t="s">
         <v>36</v>
@@ -37506,7 +37544,7 @@
         <v>7003</v>
       </c>
       <c r="B228" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C228" s="14" t="s">
         <v>36</v>
@@ -37540,7 +37578,7 @@
         <v>44012</v>
       </c>
       <c r="B229" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C229" s="14" t="s">
         <v>36</v>
@@ -37574,7 +37612,7 @@
         <v>44014</v>
       </c>
       <c r="B230" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C230" s="14" t="s">
         <v>36</v>
@@ -37608,7 +37646,7 @@
         <v>44011</v>
       </c>
       <c r="B231" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C231" s="14" t="s">
         <v>36</v>
@@ -37642,7 +37680,7 @@
         <v>44015</v>
       </c>
       <c r="B232" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C232" s="14" t="s">
         <v>36</v>
@@ -37676,7 +37714,7 @@
         <v>44005</v>
       </c>
       <c r="B233" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C233" s="14" t="s">
         <v>36</v>
@@ -37710,7 +37748,7 @@
         <v>43001</v>
       </c>
       <c r="B234" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C234" s="14" t="s">
         <v>36</v>
@@ -37744,7 +37782,7 @@
         <v>2004</v>
       </c>
       <c r="B235" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C235" s="14" t="s">
         <v>36</v>
@@ -37778,7 +37816,7 @@
         <v>2003</v>
       </c>
       <c r="B236" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C236" s="14" t="s">
         <v>36</v>
@@ -37812,7 +37850,7 @@
         <v>2002</v>
       </c>
       <c r="B237" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C237" s="14" t="s">
         <v>36</v>
@@ -37846,7 +37884,7 @@
         <v>2005</v>
       </c>
       <c r="B238" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C238" s="14" t="s">
         <v>36</v>
@@ -37880,7 +37918,7 @@
         <v>6002</v>
       </c>
       <c r="B239" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C239" s="14" t="s">
         <v>36</v>
@@ -37914,7 +37952,7 @@
         <v>6003</v>
       </c>
       <c r="B240" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C240" s="14" t="s">
         <v>36</v>
@@ -37948,7 +37986,7 @@
         <v>3</v>
       </c>
       <c r="B241" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C241" s="14" t="s">
         <v>51</v>
@@ -37982,7 +38020,7 @@
         <v>4</v>
       </c>
       <c r="B242" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C242" s="14" t="s">
         <v>51</v>
@@ -38016,7 +38054,7 @@
         <v>0</v>
       </c>
       <c r="B243" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C243" s="14" t="s">
         <v>51</v>
@@ -38050,7 +38088,7 @@
         <v>1</v>
       </c>
       <c r="B244" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C244" s="14" t="s">
         <v>51</v>
@@ -38084,7 +38122,7 @@
         <v>252</v>
       </c>
       <c r="B245" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C245" s="14" t="s">
         <v>51</v>
@@ -38118,7 +38156,7 @@
         <v>251</v>
       </c>
       <c r="B246" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C246" s="14" t="s">
         <v>51</v>
@@ -38152,7 +38190,7 @@
         <v>255</v>
       </c>
       <c r="B247" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C247" s="14" t="s">
         <v>51</v>
@@ -38186,7 +38224,7 @@
         <v>250</v>
       </c>
       <c r="B248" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C248" s="14" t="s">
         <v>51</v>
@@ -38220,7 +38258,7 @@
         <v>254</v>
       </c>
       <c r="B249" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C249" s="14" t="s">
         <v>51</v>
@@ -38254,7 +38292,7 @@
         <v>2</v>
       </c>
       <c r="B250" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C250" s="14" t="s">
         <v>51</v>
@@ -38288,7 +38326,7 @@
         <v>253</v>
       </c>
       <c r="B251" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C251" s="14" t="s">
         <v>51</v>
@@ -38322,7 +38360,7 @@
         <v>3</v>
       </c>
       <c r="B252" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C252" s="14" t="s">
         <v>22</v>
@@ -38356,7 +38394,7 @@
         <v>4</v>
       </c>
       <c r="B253" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C253" s="14" t="s">
         <v>22</v>
@@ -38390,7 +38428,7 @@
         <v>2</v>
       </c>
       <c r="B254" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C254" s="14" t="s">
         <v>22</v>
@@ -38424,7 +38462,7 @@
         <v>252</v>
       </c>
       <c r="B255" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C255" s="14" t="s">
         <v>22</v>
@@ -38458,7 +38496,7 @@
         <v>255</v>
       </c>
       <c r="B256" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C256" s="14" t="s">
         <v>22</v>
@@ -38492,7 +38530,7 @@
         <v>250</v>
       </c>
       <c r="B257" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C257" s="14" t="s">
         <v>22</v>
@@ -38526,7 +38564,7 @@
         <v>1</v>
       </c>
       <c r="B258" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C258" s="14" t="s">
         <v>22</v>
@@ -38560,10 +38598,10 @@
         <v>8</v>
       </c>
       <c r="B259" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C259" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D259" s="13"/>
       <c r="E259" s="13"/>
@@ -38594,10 +38632,10 @@
         <v>4</v>
       </c>
       <c r="B260" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C260" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D260" s="13"/>
       <c r="E260" s="13"/>
@@ -38628,10 +38666,10 @@
         <v>1</v>
       </c>
       <c r="B261" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C261" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D261" s="13"/>
       <c r="E261" s="13"/>
@@ -38662,10 +38700,10 @@
         <v>2</v>
       </c>
       <c r="B262" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C262" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D262" s="13"/>
       <c r="E262" s="13"/>
@@ -38696,10 +38734,10 @@
         <v>10</v>
       </c>
       <c r="B263" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C263" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D263" s="13"/>
       <c r="E263" s="13"/>
@@ -38730,10 +38768,10 @@
         <v>5</v>
       </c>
       <c r="B264" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C264" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D264" s="13"/>
       <c r="E264" s="13"/>
@@ -38764,10 +38802,10 @@
         <v>6</v>
       </c>
       <c r="B265" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C265" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D265" s="13"/>
       <c r="E265" s="13"/>
@@ -38798,10 +38836,10 @@
         <v>0</v>
       </c>
       <c r="B266" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C266" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D266" s="13"/>
       <c r="E266" s="13"/>
@@ -38832,10 +38870,10 @@
         <v>252</v>
       </c>
       <c r="B267" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C267" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D267" s="13"/>
       <c r="E267" s="13"/>
@@ -38866,10 +38904,10 @@
         <v>251</v>
       </c>
       <c r="B268" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C268" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D268" s="13"/>
       <c r="E268" s="13"/>
@@ -38900,10 +38938,10 @@
         <v>255</v>
       </c>
       <c r="B269" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C269" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D269" s="13"/>
       <c r="E269" s="13"/>
@@ -38934,10 +38972,10 @@
         <v>250</v>
       </c>
       <c r="B270" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C270" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D270" s="13"/>
       <c r="E270" s="13"/>
@@ -38968,10 +39006,10 @@
         <v>11</v>
       </c>
       <c r="B271" s="13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C271" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D271" s="13"/>
       <c r="E271" s="13"/>
@@ -39002,10 +39040,10 @@
         <v>3</v>
       </c>
       <c r="B272" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C272" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D272" s="13"/>
       <c r="E272" s="13"/>
@@ -39036,10 +39074,10 @@
         <v>7</v>
       </c>
       <c r="B273" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C273" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D273" s="13"/>
       <c r="E273" s="13"/>
@@ -39070,10 +39108,10 @@
         <v>9</v>
       </c>
       <c r="B274" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C274" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D274" s="13"/>
       <c r="E274" s="13"/>
@@ -39104,10 +39142,10 @@
         <v>254</v>
       </c>
       <c r="B275" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C275" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D275" s="13"/>
       <c r="E275" s="13"/>
@@ -39138,10 +39176,10 @@
         <v>253</v>
       </c>
       <c r="B276" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C276" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D276" s="13"/>
       <c r="E276" s="13"/>
@@ -39172,10 +39210,10 @@
         <v>7</v>
       </c>
       <c r="B277" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C277" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D277" s="13"/>
       <c r="E277" s="13"/>
@@ -39206,10 +39244,10 @@
         <v>2</v>
       </c>
       <c r="B278" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C278" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D278" s="13"/>
       <c r="E278" s="13"/>
@@ -39240,10 +39278,10 @@
         <v>1</v>
       </c>
       <c r="B279" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C279" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D279" s="13"/>
       <c r="E279" s="13"/>
@@ -39274,10 +39312,10 @@
         <v>3</v>
       </c>
       <c r="B280" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C280" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D280" s="13"/>
       <c r="E280" s="13"/>
@@ -39308,10 +39346,10 @@
         <v>4</v>
       </c>
       <c r="B281" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C281" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D281" s="13"/>
       <c r="E281" s="13"/>
@@ -39342,10 +39380,10 @@
         <v>15</v>
       </c>
       <c r="B282" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C282" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D282" s="13"/>
       <c r="E282" s="13"/>
@@ -39376,10 +39414,10 @@
         <v>6</v>
       </c>
       <c r="B283" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C283" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D283" s="13"/>
       <c r="E283" s="13"/>
@@ -39410,10 +39448,10 @@
         <v>16</v>
       </c>
       <c r="B284" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C284" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D284" s="13"/>
       <c r="E284" s="13"/>
@@ -39444,10 +39482,10 @@
         <v>5</v>
       </c>
       <c r="B285" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C285" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D285" s="13"/>
       <c r="E285" s="13"/>
@@ -39478,10 +39516,10 @@
         <v>13</v>
       </c>
       <c r="B286" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C286" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D286" s="13"/>
       <c r="E286" s="13"/>
@@ -39512,10 +39550,10 @@
         <v>252</v>
       </c>
       <c r="B287" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C287" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D287" s="13"/>
       <c r="E287" s="13"/>
@@ -39546,10 +39584,10 @@
         <v>251</v>
       </c>
       <c r="B288" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C288" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D288" s="13"/>
       <c r="E288" s="13"/>
@@ -39580,10 +39618,10 @@
         <v>255</v>
       </c>
       <c r="B289" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C289" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D289" s="13"/>
       <c r="E289" s="13"/>
@@ -39614,10 +39652,10 @@
         <v>9</v>
       </c>
       <c r="B290" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C290" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D290" s="13"/>
       <c r="E290" s="13"/>
@@ -39648,10 +39686,10 @@
         <v>250</v>
       </c>
       <c r="B291" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C291" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D291" s="13"/>
       <c r="E291" s="13"/>
@@ -39682,10 +39720,10 @@
         <v>10</v>
       </c>
       <c r="B292" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C292" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D292" s="13"/>
       <c r="E292" s="13"/>
@@ -39716,10 +39754,10 @@
         <v>11</v>
       </c>
       <c r="B293" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C293" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D293" s="13"/>
       <c r="E293" s="13"/>
@@ -39750,10 +39788,10 @@
         <v>14</v>
       </c>
       <c r="B294" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C294" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D294" s="13"/>
       <c r="E294" s="13"/>
@@ -39784,10 +39822,10 @@
         <v>254</v>
       </c>
       <c r="B295" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C295" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D295" s="13"/>
       <c r="E295" s="13"/>
@@ -39818,10 +39856,10 @@
         <v>253</v>
       </c>
       <c r="B296" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C296" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D296" s="13"/>
       <c r="E296" s="13"/>
@@ -39852,10 +39890,10 @@
         <v>8</v>
       </c>
       <c r="B297" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C297" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D297" s="13"/>
       <c r="E297" s="13"/>
@@ -39886,10 +39924,10 @@
         <v>12</v>
       </c>
       <c r="B298" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C298" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D298" s="13"/>
       <c r="E298" s="13"/>
@@ -39920,10 +39958,10 @@
         <v>1</v>
       </c>
       <c r="B299" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C299" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D299" s="13"/>
       <c r="E299" s="13"/>
@@ -39954,10 +39992,10 @@
         <v>6</v>
       </c>
       <c r="B300" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C300" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D300" s="13"/>
       <c r="E300" s="13"/>
@@ -39988,10 +40026,10 @@
         <v>5</v>
       </c>
       <c r="B301" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C301" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D301" s="13"/>
       <c r="E301" s="13"/>
@@ -40022,10 +40060,10 @@
         <v>4</v>
       </c>
       <c r="B302" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C302" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D302" s="13"/>
       <c r="E302" s="13"/>
@@ -40056,10 +40094,10 @@
         <v>3</v>
       </c>
       <c r="B303" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C303" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D303" s="13"/>
       <c r="E303" s="13"/>
@@ -40090,10 +40128,10 @@
         <v>2</v>
       </c>
       <c r="B304" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C304" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D304" s="13"/>
       <c r="E304" s="13"/>
@@ -40124,10 +40162,10 @@
         <v>23</v>
       </c>
       <c r="B305" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C305" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D305" s="13"/>
       <c r="E305" s="13"/>
@@ -40158,10 +40196,10 @@
         <v>24</v>
       </c>
       <c r="B306" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C306" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D306" s="13"/>
       <c r="E306" s="13"/>
@@ -40192,10 +40230,10 @@
         <v>25</v>
       </c>
       <c r="B307" s="13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C307" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D307" s="13"/>
       <c r="E307" s="13"/>
@@ -40226,10 +40264,10 @@
         <v>14</v>
       </c>
       <c r="B308" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C308" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D308" s="13"/>
       <c r="E308" s="13"/>
@@ -40260,10 +40298,10 @@
         <v>26</v>
       </c>
       <c r="B309" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C309" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D309" s="13"/>
       <c r="E309" s="13"/>
@@ -40294,10 +40332,10 @@
         <v>22</v>
       </c>
       <c r="B310" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C310" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D310" s="13"/>
       <c r="E310" s="13"/>
@@ -40328,10 +40366,10 @@
         <v>15</v>
       </c>
       <c r="B311" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C311" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D311" s="13"/>
       <c r="E311" s="13"/>
@@ -40362,10 +40400,10 @@
         <v>17</v>
       </c>
       <c r="B312" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C312" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D312" s="13"/>
       <c r="E312" s="13"/>
@@ -40396,10 +40434,10 @@
         <v>16</v>
       </c>
       <c r="B313" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C313" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D313" s="13"/>
       <c r="E313" s="13"/>
@@ -40430,10 +40468,10 @@
         <v>13</v>
       </c>
       <c r="B314" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C314" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D314" s="13"/>
       <c r="E314" s="13"/>
@@ -40464,10 +40502,10 @@
         <v>252</v>
       </c>
       <c r="B315" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C315" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D315" s="13"/>
       <c r="E315" s="13"/>
@@ -40498,10 +40536,10 @@
         <v>251</v>
       </c>
       <c r="B316" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C316" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D316" s="13"/>
       <c r="E316" s="13"/>
@@ -40532,10 +40570,10 @@
         <v>255</v>
       </c>
       <c r="B317" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C317" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D317" s="13"/>
       <c r="E317" s="13"/>
@@ -40566,10 +40604,10 @@
         <v>250</v>
       </c>
       <c r="B318" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C318" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D318" s="13"/>
       <c r="E318" s="13"/>
@@ -40600,10 +40638,10 @@
         <v>10</v>
       </c>
       <c r="B319" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C319" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D319" s="13"/>
       <c r="E319" s="13"/>
@@ -40634,10 +40672,10 @@
         <v>11</v>
       </c>
       <c r="B320" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C320" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D320" s="13"/>
       <c r="E320" s="13"/>
@@ -40668,10 +40706,10 @@
         <v>12</v>
       </c>
       <c r="B321" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C321" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D321" s="13"/>
       <c r="E321" s="13"/>
@@ -40702,10 +40740,10 @@
         <v>7</v>
       </c>
       <c r="B322" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C322" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D322" s="13"/>
       <c r="E322" s="13"/>
@@ -40736,10 +40774,10 @@
         <v>8</v>
       </c>
       <c r="B323" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C323" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D323" s="13"/>
       <c r="E323" s="13"/>
@@ -40770,10 +40808,10 @@
         <v>9</v>
       </c>
       <c r="B324" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C324" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D324" s="13"/>
       <c r="E324" s="13"/>
@@ -40804,10 +40842,10 @@
         <v>18</v>
       </c>
       <c r="B325" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C325" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D325" s="13"/>
       <c r="E325" s="13"/>
@@ -40838,10 +40876,10 @@
         <v>20</v>
       </c>
       <c r="B326" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C326" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D326" s="13"/>
       <c r="E326" s="13"/>
@@ -40872,10 +40910,10 @@
         <v>19</v>
       </c>
       <c r="B327" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C327" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D327" s="13"/>
       <c r="E327" s="13"/>
@@ -40906,10 +40944,10 @@
         <v>254</v>
       </c>
       <c r="B328" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C328" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D328" s="13"/>
       <c r="E328" s="13"/>
@@ -40940,10 +40978,10 @@
         <v>253</v>
       </c>
       <c r="B329" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C329" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D329" s="13"/>
       <c r="E329" s="13"/>
@@ -40974,10 +41012,10 @@
         <v>21</v>
       </c>
       <c r="B330" s="13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C330" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D330" s="13"/>
       <c r="E330" s="13"/>
@@ -41008,10 +41046,10 @@
         <v>1</v>
       </c>
       <c r="B331" s="16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C331" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D331" s="13"/>
       <c r="E331" s="13"/>
@@ -41042,10 +41080,10 @@
         <v>2</v>
       </c>
       <c r="B332" s="16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C332" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D332" s="13"/>
       <c r="E332" s="13"/>
@@ -41076,10 +41114,10 @@
         <v>251</v>
       </c>
       <c r="B333" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C333" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D333" s="13"/>
       <c r="E333" s="13"/>

</xml_diff>

<commit_message>
fixes enumeration in release metadata xlsx
</commit_message>
<xml_diff>
--- a/data-raw/metadata/camp_release_metadata.xlsx
+++ b/data-raw/metadata/camp_release_metadata.xlsx
@@ -8,16 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E3D5C0-4E04-F24F-B870-D62B2BF45C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FD9DA7-8C16-3E43-BA9B-CA04375C9CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68640" yWindow="-12120" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
     <sheet name="code_definitions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mit2xqhZQrvV/jMm32OR1tEBu8z4A=="/>
     </ext>
@@ -26,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="316">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -122,9 +133,6 @@
   </si>
   <si>
     <t>Origin or production type of fish marked</t>
-  </si>
-  <si>
-    <t>sourceofFishSiteID</t>
   </si>
   <si>
     <t>Site where fish used for release were from</t>
@@ -994,23 +1002,27 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1090,11 +1102,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1313,7 +1325,7 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1655,10 +1667,10 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
@@ -1693,10 +1705,10 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
@@ -1731,10 +1743,10 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>15</v>
@@ -1769,28 +1781,28 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="3"/>
@@ -1817,28 +1829,28 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="3"/>
@@ -1865,28 +1877,28 @@
     </row>
     <row r="14" spans="1:26" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="3"/>
@@ -1913,33 +1925,33 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="2"/>
       <c r="J15" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K15" s="2"/>
-      <c r="L15" s="19" t="s">
+      <c r="L15" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="M15" s="17" t="s">
         <v>315</v>
-      </c>
-      <c r="M15" s="19" t="s">
-        <v>316</v>
       </c>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1957,10 +1969,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>
@@ -1995,28 +2007,28 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="3"/>
@@ -2043,10 +2055,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
@@ -2081,10 +2093,10 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
@@ -2119,10 +2131,10 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>15</v>
@@ -2157,10 +2169,10 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>15</v>
@@ -2195,19 +2207,19 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -2792,7 +2804,7 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="17"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="2"/>
@@ -2820,7 +2832,7 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="18"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="2"/>
@@ -2848,7 +2860,7 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="17"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="2"/>
@@ -2876,7 +2888,7 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="2"/>
@@ -29811,7 +29823,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -29823,13 +29837,13 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>67</v>
       </c>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
@@ -29860,7 +29874,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>13</v>
@@ -29894,7 +29908,7 @@
         <v>159697</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>24</v>
@@ -29928,7 +29942,7 @@
         <v>159698</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>24</v>
@@ -29962,7 +29976,7 @@
         <v>159700</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>24</v>
@@ -29996,7 +30010,7 @@
         <v>159707</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>24</v>
@@ -30030,7 +30044,7 @@
         <v>159709</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>24</v>
@@ -30064,7 +30078,7 @@
         <v>159710</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>24</v>
@@ -30098,7 +30112,7 @@
         <v>159713</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>24</v>
@@ -30132,7 +30146,7 @@
         <v>161030</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>24</v>
@@ -30166,7 +30180,7 @@
         <v>161064</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>24</v>
@@ -30200,7 +30214,7 @@
         <v>161067</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>24</v>
@@ -30234,7 +30248,7 @@
         <v>161068</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>24</v>
@@ -30268,7 +30282,7 @@
         <v>161127</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>24</v>
@@ -30302,7 +30316,7 @@
         <v>161702</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>24</v>
@@ -30336,7 +30350,7 @@
         <v>161738</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>24</v>
@@ -30370,7 +30384,7 @@
         <v>161931</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>24</v>
@@ -30404,7 +30418,7 @@
         <v>161974</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>24</v>
@@ -30438,7 +30452,7 @@
         <v>161975</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>24</v>
@@ -30472,7 +30486,7 @@
         <v>161977</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>24</v>
@@ -30506,7 +30520,7 @@
         <v>161979</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>24</v>
@@ -30540,7 +30554,7 @@
         <v>161980</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>24</v>
@@ -30574,7 +30588,7 @@
         <v>161989</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>24</v>
@@ -30608,7 +30622,7 @@
         <v>161997</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C24" s="14" t="s">
         <v>24</v>
@@ -30642,7 +30656,7 @@
         <v>162003</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>24</v>
@@ -30676,7 +30690,7 @@
         <v>162032</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>24</v>
@@ -30710,7 +30724,7 @@
         <v>162033</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C27" s="14" t="s">
         <v>24</v>
@@ -30744,7 +30758,7 @@
         <v>163342</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>24</v>
@@ -30778,7 +30792,7 @@
         <v>163344</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>24</v>
@@ -30812,7 +30826,7 @@
         <v>163350</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C30" s="14" t="s">
         <v>24</v>
@@ -30846,7 +30860,7 @@
         <v>163368</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>24</v>
@@ -30880,7 +30894,7 @@
         <v>163387</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>24</v>
@@ -30914,7 +30928,7 @@
         <v>163517</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>24</v>
@@ -30948,7 +30962,7 @@
         <v>163524</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>24</v>
@@ -30982,7 +30996,7 @@
         <v>163565</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>24</v>
@@ -31016,7 +31030,7 @@
         <v>163569</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>24</v>
@@ -31050,7 +31064,7 @@
         <v>163587</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C37" s="14" t="s">
         <v>24</v>
@@ -31084,7 +31098,7 @@
         <v>163589</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>24</v>
@@ -31118,7 +31132,7 @@
         <v>163603</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>24</v>
@@ -31152,7 +31166,7 @@
         <v>163792</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C40" s="14" t="s">
         <v>24</v>
@@ -31186,7 +31200,7 @@
         <v>163892</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>24</v>
@@ -31220,7 +31234,7 @@
         <v>163908</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>24</v>
@@ -31254,7 +31268,7 @@
         <v>163995</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>24</v>
@@ -31288,7 +31302,7 @@
         <v>163998</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>24</v>
@@ -31322,7 +31336,7 @@
         <v>164034</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>24</v>
@@ -31356,7 +31370,7 @@
         <v>164037</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>24</v>
@@ -31390,7 +31404,7 @@
         <v>164039</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>24</v>
@@ -31424,7 +31438,7 @@
         <v>164041</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>24</v>
@@ -31458,7 +31472,7 @@
         <v>164043</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C49" s="14" t="s">
         <v>24</v>
@@ -31492,7 +31506,7 @@
         <v>165679</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C50" s="14" t="s">
         <v>24</v>
@@ -31526,7 +31540,7 @@
         <v>165877</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C51" s="14" t="s">
         <v>24</v>
@@ -31560,7 +31574,7 @@
         <v>165878</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C52" s="14" t="s">
         <v>24</v>
@@ -31594,7 +31608,7 @@
         <v>165993</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C53" s="14" t="s">
         <v>24</v>
@@ -31628,7 +31642,7 @@
         <v>165998</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C54" s="14" t="s">
         <v>24</v>
@@ -31662,7 +31676,7 @@
         <v>166365</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C55" s="14" t="s">
         <v>24</v>
@@ -31696,7 +31710,7 @@
         <v>167229</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C56" s="14" t="s">
         <v>24</v>
@@ -31730,7 +31744,7 @@
         <v>167233</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C57" s="14" t="s">
         <v>24</v>
@@ -31764,7 +31778,7 @@
         <v>167234</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C58" s="14" t="s">
         <v>24</v>
@@ -31798,7 +31812,7 @@
         <v>167680</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C59" s="14" t="s">
         <v>24</v>
@@ -31832,7 +31846,7 @@
         <v>168093</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>24</v>
@@ -31866,7 +31880,7 @@
         <v>168130</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C61" s="14" t="s">
         <v>24</v>
@@ -31900,7 +31914,7 @@
         <v>168132</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>24</v>
@@ -31934,7 +31948,7 @@
         <v>168139</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C63" s="14" t="s">
         <v>24</v>
@@ -31968,7 +31982,7 @@
         <v>168141</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C64" s="14" t="s">
         <v>24</v>
@@ -32002,7 +32016,7 @@
         <v>168144</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C65" s="14" t="s">
         <v>24</v>
@@ -32036,7 +32050,7 @@
         <v>168154</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C66" s="14" t="s">
         <v>24</v>
@@ -32070,7 +32084,7 @@
         <v>168158</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C67" s="14" t="s">
         <v>24</v>
@@ -32104,7 +32118,7 @@
         <v>168160</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C68" s="14" t="s">
         <v>24</v>
@@ -32138,7 +32152,7 @@
         <v>168161</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C69" s="14" t="s">
         <v>24</v>
@@ -32172,7 +32186,7 @@
         <v>168163</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C70" s="14" t="s">
         <v>24</v>
@@ -32206,7 +32220,7 @@
         <v>168165</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C71" s="14" t="s">
         <v>24</v>
@@ -32240,7 +32254,7 @@
         <v>168166</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C72" s="14" t="s">
         <v>24</v>
@@ -32274,7 +32288,7 @@
         <v>168167</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>24</v>
@@ -32308,7 +32322,7 @@
         <v>168175</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C74" s="14" t="s">
         <v>24</v>
@@ -32342,7 +32356,7 @@
         <v>168487</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>24</v>
@@ -32376,7 +32390,7 @@
         <v>171882</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C76" s="14" t="s">
         <v>24</v>
@@ -32410,7 +32424,7 @@
         <v>250</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C77" s="14" t="s">
         <v>24</v>
@@ -32444,7 +32458,7 @@
         <v>251</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C78" s="14" t="s">
         <v>24</v>
@@ -32478,7 +32492,7 @@
         <v>252</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C79" s="14" t="s">
         <v>24</v>
@@ -32512,7 +32526,7 @@
         <v>253</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C80" s="14" t="s">
         <v>24</v>
@@ -32546,7 +32560,7 @@
         <v>254</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C81" s="14" t="s">
         <v>24</v>
@@ -32580,7 +32594,7 @@
         <v>255</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C82" s="14" t="s">
         <v>24</v>
@@ -32614,7 +32628,7 @@
         <v>550562</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C83" s="14" t="s">
         <v>24</v>
@@ -32648,7 +32662,7 @@
         <v>553322</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C84" s="14" t="s">
         <v>24</v>
@@ -32682,7 +32696,7 @@
         <v>622248</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C85" s="14" t="s">
         <v>24</v>
@@ -32716,7 +32730,7 @@
         <v>3</v>
       </c>
       <c r="B86" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C86" s="14" t="s">
         <v>26</v>
@@ -32750,7 +32764,7 @@
         <v>5</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C87" s="14" t="s">
         <v>26</v>
@@ -32784,7 +32798,7 @@
         <v>6</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C88" s="14" t="s">
         <v>26</v>
@@ -32818,7 +32832,7 @@
         <v>252</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C89" s="14" t="s">
         <v>26</v>
@@ -32852,7 +32866,7 @@
         <v>251</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C90" s="14" t="s">
         <v>26</v>
@@ -32886,7 +32900,7 @@
         <v>255</v>
       </c>
       <c r="B91" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C91" s="14" t="s">
         <v>26</v>
@@ -32920,7 +32934,7 @@
         <v>250</v>
       </c>
       <c r="B92" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C92" s="14" t="s">
         <v>26</v>
@@ -32954,7 +32968,7 @@
         <v>254</v>
       </c>
       <c r="B93" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C93" s="14" t="s">
         <v>26</v>
@@ -32988,7 +33002,7 @@
         <v>1</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C94" s="14" t="s">
         <v>26</v>
@@ -33022,7 +33036,7 @@
         <v>2</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C95" s="14" t="s">
         <v>26</v>
@@ -33056,7 +33070,7 @@
         <v>253</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C96" s="14" t="s">
         <v>26</v>
@@ -33090,7 +33104,7 @@
         <v>4</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C97" s="14" t="s">
         <v>26</v>
@@ -33124,7 +33138,7 @@
         <v>11</v>
       </c>
       <c r="B98" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C98" s="14" t="s">
         <v>28</v>
@@ -33158,7 +33172,7 @@
         <v>6</v>
       </c>
       <c r="B99" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C99" s="14" t="s">
         <v>28</v>
@@ -33192,7 +33206,7 @@
         <v>12</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C100" s="14" t="s">
         <v>28</v>
@@ -33226,7 +33240,7 @@
         <v>17</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C101" s="14" t="s">
         <v>28</v>
@@ -33260,7 +33274,7 @@
         <v>3</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C102" s="14" t="s">
         <v>28</v>
@@ -33294,7 +33308,7 @@
         <v>15</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C103" s="14" t="s">
         <v>28</v>
@@ -33328,7 +33342,7 @@
         <v>10</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C104" s="14" t="s">
         <v>28</v>
@@ -33362,7 +33376,7 @@
         <v>16</v>
       </c>
       <c r="B105" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C105" s="14" t="s">
         <v>28</v>
@@ -33396,7 +33410,7 @@
         <v>13</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C106" s="14" t="s">
         <v>28</v>
@@ -33430,7 +33444,7 @@
         <v>14</v>
       </c>
       <c r="B107" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C107" s="14" t="s">
         <v>28</v>
@@ -33464,7 +33478,7 @@
         <v>252</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C108" s="14" t="s">
         <v>28</v>
@@ -33498,7 +33512,7 @@
         <v>251</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C109" s="14" t="s">
         <v>28</v>
@@ -33532,7 +33546,7 @@
         <v>255</v>
       </c>
       <c r="B110" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C110" s="14" t="s">
         <v>28</v>
@@ -33566,7 +33580,7 @@
         <v>250</v>
       </c>
       <c r="B111" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C111" s="14" t="s">
         <v>28</v>
@@ -33600,7 +33614,7 @@
         <v>4</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C112" s="14" t="s">
         <v>28</v>
@@ -33634,7 +33648,7 @@
         <v>7</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C113" s="14" t="s">
         <v>28</v>
@@ -33668,7 +33682,7 @@
         <v>19</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C114" s="14" t="s">
         <v>28</v>
@@ -33702,7 +33716,7 @@
         <v>254</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C115" s="14" t="s">
         <v>28</v>
@@ -33736,7 +33750,7 @@
         <v>5</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C116" s="14" t="s">
         <v>28</v>
@@ -33770,7 +33784,7 @@
         <v>8</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C117" s="14" t="s">
         <v>28</v>
@@ -33804,7 +33818,7 @@
         <v>20</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C118" s="14" t="s">
         <v>28</v>
@@ -33838,7 +33852,7 @@
         <v>18</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C119" s="14" t="s">
         <v>28</v>
@@ -33872,7 +33886,7 @@
         <v>253</v>
       </c>
       <c r="B120" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C120" s="14" t="s">
         <v>28</v>
@@ -33906,7 +33920,7 @@
         <v>9</v>
       </c>
       <c r="B121" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C121" s="14" t="s">
         <v>28</v>
@@ -33940,7 +33954,7 @@
         <v>1</v>
       </c>
       <c r="B122" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C122" s="14" t="s">
         <v>28</v>
@@ -33974,7 +33988,7 @@
         <v>2</v>
       </c>
       <c r="B123" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C123" s="14" t="s">
         <v>28</v>
@@ -34008,7 +34022,7 @@
         <v>1</v>
       </c>
       <c r="B124" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C124" s="14" t="s">
         <v>30</v>
@@ -34042,7 +34056,7 @@
         <v>3</v>
       </c>
       <c r="B125" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C125" s="14" t="s">
         <v>30</v>
@@ -34076,7 +34090,7 @@
         <v>2</v>
       </c>
       <c r="B126" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C126" s="14" t="s">
         <v>30</v>
@@ -34110,7 +34124,7 @@
         <v>252</v>
       </c>
       <c r="B127" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C127" s="14" t="s">
         <v>30</v>
@@ -34144,7 +34158,7 @@
         <v>251</v>
       </c>
       <c r="B128" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C128" s="14" t="s">
         <v>30</v>
@@ -34178,7 +34192,7 @@
         <v>255</v>
       </c>
       <c r="B129" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C129" s="14" t="s">
         <v>30</v>
@@ -34212,7 +34226,7 @@
         <v>250</v>
       </c>
       <c r="B130" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C130" s="14" t="s">
         <v>30</v>
@@ -34246,7 +34260,7 @@
         <v>254</v>
       </c>
       <c r="B131" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C131" s="14" t="s">
         <v>30</v>
@@ -34280,7 +34294,7 @@
         <v>253</v>
       </c>
       <c r="B132" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C132" s="14" t="s">
         <v>30</v>
@@ -34314,10 +34328,10 @@
         <v>3000</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="C133" s="14" t="s">
-        <v>32</v>
+        <v>178</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D133" s="13"/>
       <c r="E133" s="13"/>
@@ -34348,10 +34362,10 @@
         <v>44000</v>
       </c>
       <c r="B134" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="C134" s="14" t="s">
-        <v>32</v>
+        <v>179</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D134" s="13"/>
       <c r="E134" s="13"/>
@@ -34382,10 +34396,10 @@
         <v>52000</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="C135" s="14" t="s">
-        <v>32</v>
+        <v>180</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D135" s="13"/>
       <c r="E135" s="13"/>
@@ -34416,10 +34430,10 @@
         <v>51000</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="C136" s="14" t="s">
-        <v>32</v>
+        <v>181</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D136" s="13"/>
       <c r="E136" s="13"/>
@@ -34450,10 +34464,10 @@
         <v>5000</v>
       </c>
       <c r="B137" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="C137" s="14" t="s">
-        <v>32</v>
+        <v>182</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D137" s="13"/>
       <c r="E137" s="13"/>
@@ -34484,10 +34498,10 @@
         <v>46000</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="C138" s="14" t="s">
-        <v>32</v>
+        <v>183</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D138" s="13"/>
       <c r="E138" s="13"/>
@@ -34518,10 +34532,10 @@
         <v>4000</v>
       </c>
       <c r="B139" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="C139" s="14" t="s">
-        <v>32</v>
+        <v>184</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D139" s="13"/>
       <c r="E139" s="13"/>
@@ -34552,10 +34566,10 @@
         <v>45000</v>
       </c>
       <c r="B140" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="C140" s="14" t="s">
-        <v>32</v>
+        <v>185</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D140" s="13"/>
       <c r="E140" s="13"/>
@@ -34586,10 +34600,10 @@
         <v>252</v>
       </c>
       <c r="B141" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="C141" s="14" t="s">
-        <v>32</v>
+        <v>186</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D141" s="13"/>
       <c r="E141" s="13"/>
@@ -34620,10 +34634,10 @@
         <v>251</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="C142" s="14" t="s">
-        <v>32</v>
+        <v>143</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D142" s="13"/>
       <c r="E142" s="13"/>
@@ -34654,10 +34668,10 @@
         <v>255</v>
       </c>
       <c r="B143" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="C143" s="14" t="s">
-        <v>32</v>
+        <v>147</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D143" s="13"/>
       <c r="E143" s="13"/>
@@ -34688,10 +34702,10 @@
         <v>53000</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="C144" s="14" t="s">
-        <v>32</v>
+        <v>187</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D144" s="13"/>
       <c r="E144" s="13"/>
@@ -34722,10 +34736,10 @@
         <v>54000</v>
       </c>
       <c r="B145" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="C145" s="14" t="s">
-        <v>32</v>
+        <v>188</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D145" s="13"/>
       <c r="E145" s="13"/>
@@ -34756,10 +34770,10 @@
         <v>55000</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="C146" s="14" t="s">
-        <v>32</v>
+        <v>189</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D146" s="13"/>
       <c r="E146" s="13"/>
@@ -34790,10 +34804,10 @@
         <v>56000</v>
       </c>
       <c r="B147" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="C147" s="14" t="s">
-        <v>32</v>
+        <v>190</v>
+      </c>
+      <c r="C147" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D147" s="13"/>
       <c r="E147" s="13"/>
@@ -34824,10 +34838,10 @@
         <v>50000</v>
       </c>
       <c r="B148" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="C148" s="14" t="s">
-        <v>32</v>
+        <v>191</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D148" s="13"/>
       <c r="E148" s="13"/>
@@ -34858,10 +34872,10 @@
         <v>7000</v>
       </c>
       <c r="B149" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="C149" s="14" t="s">
-        <v>32</v>
+        <v>192</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D149" s="13"/>
       <c r="E149" s="13"/>
@@ -34892,10 +34906,10 @@
         <v>2000</v>
       </c>
       <c r="B150" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="C150" s="14" t="s">
-        <v>32</v>
+        <v>193</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D150" s="13"/>
       <c r="E150" s="13"/>
@@ -34926,10 +34940,10 @@
         <v>43000</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="C151" s="14" t="s">
-        <v>32</v>
+        <v>194</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D151" s="13"/>
       <c r="E151" s="13"/>
@@ -34960,10 +34974,10 @@
         <v>6000</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="C152" s="14" t="s">
-        <v>32</v>
+        <v>195</v>
+      </c>
+      <c r="C152" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D152" s="13"/>
       <c r="E152" s="13"/>
@@ -34994,10 +35008,10 @@
         <v>47000</v>
       </c>
       <c r="B153" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="C153" s="14" t="s">
-        <v>32</v>
+        <v>196</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D153" s="13"/>
       <c r="E153" s="13"/>
@@ -35028,10 +35042,10 @@
         <v>90000</v>
       </c>
       <c r="B154" s="13" t="s">
-        <v>198</v>
-      </c>
-      <c r="C154" s="14" t="s">
-        <v>32</v>
+        <v>197</v>
+      </c>
+      <c r="C154" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D154" s="13"/>
       <c r="E154" s="13"/>
@@ -35062,10 +35076,10 @@
         <v>253</v>
       </c>
       <c r="B155" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="C155" s="14" t="s">
-        <v>32</v>
+        <v>145</v>
+      </c>
+      <c r="C155" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D155" s="13"/>
       <c r="E155" s="13"/>
@@ -35096,10 +35110,10 @@
         <v>3000</v>
       </c>
       <c r="B156" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D156" s="13"/>
       <c r="E156" s="13"/>
@@ -35130,10 +35144,10 @@
         <v>44000</v>
       </c>
       <c r="B157" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D157" s="13"/>
       <c r="E157" s="13"/>
@@ -35164,10 +35178,10 @@
         <v>52000</v>
       </c>
       <c r="B158" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C158" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D158" s="13"/>
       <c r="E158" s="13"/>
@@ -35198,10 +35212,10 @@
         <v>51000</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D159" s="13"/>
       <c r="E159" s="13"/>
@@ -35232,10 +35246,10 @@
         <v>5000</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C160" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D160" s="13"/>
       <c r="E160" s="13"/>
@@ -35266,10 +35280,10 @@
         <v>46000</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C161" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D161" s="13"/>
       <c r="E161" s="13"/>
@@ -35300,10 +35314,10 @@
         <v>4000</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C162" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D162" s="13"/>
       <c r="E162" s="13"/>
@@ -35334,10 +35348,10 @@
         <v>45000</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C163" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D163" s="13"/>
       <c r="E163" s="13"/>
@@ -35368,10 +35382,10 @@
         <v>252</v>
       </c>
       <c r="B164" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C164" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D164" s="13"/>
       <c r="E164" s="13"/>
@@ -35402,10 +35416,10 @@
         <v>251</v>
       </c>
       <c r="B165" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C165" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D165" s="13"/>
       <c r="E165" s="13"/>
@@ -35436,10 +35450,10 @@
         <v>255</v>
       </c>
       <c r="B166" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C166" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D166" s="13"/>
       <c r="E166" s="13"/>
@@ -35470,10 +35484,10 @@
         <v>53000</v>
       </c>
       <c r="B167" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C167" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D167" s="13"/>
       <c r="E167" s="13"/>
@@ -35504,10 +35518,10 @@
         <v>54000</v>
       </c>
       <c r="B168" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C168" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D168" s="13"/>
       <c r="E168" s="13"/>
@@ -35538,10 +35552,10 @@
         <v>55000</v>
       </c>
       <c r="B169" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C169" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D169" s="13"/>
       <c r="E169" s="13"/>
@@ -35572,10 +35586,10 @@
         <v>56000</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C170" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D170" s="13"/>
       <c r="E170" s="13"/>
@@ -35606,10 +35620,10 @@
         <v>50000</v>
       </c>
       <c r="B171" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C171" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D171" s="13"/>
       <c r="E171" s="13"/>
@@ -35640,10 +35654,10 @@
         <v>7000</v>
       </c>
       <c r="B172" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C172" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D172" s="13"/>
       <c r="E172" s="13"/>
@@ -35674,10 +35688,10 @@
         <v>2000</v>
       </c>
       <c r="B173" s="13" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C173" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D173" s="13"/>
       <c r="E173" s="13"/>
@@ -35708,10 +35722,10 @@
         <v>43000</v>
       </c>
       <c r="B174" s="13" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C174" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D174" s="13"/>
       <c r="E174" s="13"/>
@@ -35742,10 +35756,10 @@
         <v>6000</v>
       </c>
       <c r="B175" s="13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C175" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D175" s="13"/>
       <c r="E175" s="13"/>
@@ -35776,10 +35790,10 @@
         <v>47000</v>
       </c>
       <c r="B176" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C176" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D176" s="13"/>
       <c r="E176" s="13"/>
@@ -35810,10 +35824,10 @@
         <v>90000</v>
       </c>
       <c r="B177" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C177" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D177" s="13"/>
       <c r="E177" s="13"/>
@@ -35844,10 +35858,10 @@
         <v>253</v>
       </c>
       <c r="B178" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C178" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D178" s="13"/>
       <c r="E178" s="13"/>
@@ -35878,10 +35892,10 @@
         <v>2001</v>
       </c>
       <c r="B179" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C179" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D179" s="13"/>
       <c r="E179" s="13"/>
@@ -35912,10 +35926,10 @@
         <v>44018</v>
       </c>
       <c r="B180" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C180" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D180" s="13"/>
       <c r="E180" s="13"/>
@@ -35946,10 +35960,10 @@
         <v>44007</v>
       </c>
       <c r="B181" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C181" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D181" s="13"/>
       <c r="E181" s="13"/>
@@ -35980,10 +35994,10 @@
         <v>44017</v>
       </c>
       <c r="B182" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C182" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D182" s="13"/>
       <c r="E182" s="13"/>
@@ -36014,10 +36028,10 @@
         <v>44016</v>
       </c>
       <c r="B183" s="13" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C183" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D183" s="13"/>
       <c r="E183" s="13"/>
@@ -36048,10 +36062,10 @@
         <v>44013</v>
       </c>
       <c r="B184" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C184" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D184" s="13"/>
       <c r="E184" s="13"/>
@@ -36082,10 +36096,10 @@
         <v>3001</v>
       </c>
       <c r="B185" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C185" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D185" s="13"/>
       <c r="E185" s="13"/>
@@ -36116,10 +36130,10 @@
         <v>3002</v>
       </c>
       <c r="B186" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C186" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D186" s="13"/>
       <c r="E186" s="13"/>
@@ -36150,10 +36164,10 @@
         <v>52003</v>
       </c>
       <c r="B187" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C187" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D187" s="13"/>
       <c r="E187" s="13"/>
@@ -36184,10 +36198,10 @@
         <v>51002</v>
       </c>
       <c r="B188" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C188" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D188" s="13"/>
       <c r="E188" s="13"/>
@@ -36218,10 +36232,10 @@
         <v>51003</v>
       </c>
       <c r="B189" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C189" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D189" s="13"/>
       <c r="E189" s="13"/>
@@ -36252,10 +36266,10 @@
         <v>52001</v>
       </c>
       <c r="B190" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C190" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D190" s="13"/>
       <c r="E190" s="13"/>
@@ -36286,10 +36300,10 @@
         <v>52002</v>
       </c>
       <c r="B191" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C191" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D191" s="13"/>
       <c r="E191" s="13"/>
@@ -36320,10 +36334,10 @@
         <v>52004</v>
       </c>
       <c r="B192" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C192" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D192" s="13"/>
       <c r="E192" s="13"/>
@@ -36354,10 +36368,10 @@
         <v>90001</v>
       </c>
       <c r="B193" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C193" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D193" s="13"/>
       <c r="E193" s="13"/>
@@ -36388,10 +36402,10 @@
         <v>46003</v>
       </c>
       <c r="B194" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C194" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D194" s="13"/>
       <c r="E194" s="13"/>
@@ -36422,10 +36436,10 @@
         <v>46001</v>
       </c>
       <c r="B195" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C195" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D195" s="13"/>
       <c r="E195" s="13"/>
@@ -36456,10 +36470,10 @@
         <v>46004</v>
       </c>
       <c r="B196" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C196" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D196" s="13"/>
       <c r="E196" s="13"/>
@@ -36490,10 +36504,10 @@
         <v>5001</v>
       </c>
       <c r="B197" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C197" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D197" s="13"/>
       <c r="E197" s="13"/>
@@ -36524,10 +36538,10 @@
         <v>5003</v>
       </c>
       <c r="B198" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C198" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D198" s="13"/>
       <c r="E198" s="13"/>
@@ -36558,10 +36572,10 @@
         <v>5002</v>
       </c>
       <c r="B199" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C199" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D199" s="13"/>
       <c r="E199" s="13"/>
@@ -36592,10 +36606,10 @@
         <v>4001</v>
       </c>
       <c r="B200" s="13" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C200" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D200" s="13"/>
       <c r="E200" s="13"/>
@@ -36626,10 +36640,10 @@
         <v>4002</v>
       </c>
       <c r="B201" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C201" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D201" s="13"/>
       <c r="E201" s="13"/>
@@ -36660,10 +36674,10 @@
         <v>44010</v>
       </c>
       <c r="B202" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C202" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D202" s="13"/>
       <c r="E202" s="13"/>
@@ -36694,10 +36708,10 @@
         <v>51001</v>
       </c>
       <c r="B203" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C203" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D203" s="13"/>
       <c r="E203" s="13"/>
@@ -36728,10 +36742,10 @@
         <v>46002</v>
       </c>
       <c r="B204" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C204" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D204" s="13"/>
       <c r="E204" s="13"/>
@@ -36762,10 +36776,10 @@
         <v>43000</v>
       </c>
       <c r="B205" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C205" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D205" s="13"/>
       <c r="E205" s="13"/>
@@ -36796,10 +36810,10 @@
         <v>44000</v>
       </c>
       <c r="B206" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C206" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D206" s="13"/>
       <c r="E206" s="13"/>
@@ -36830,10 +36844,10 @@
         <v>45000</v>
       </c>
       <c r="B207" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C207" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D207" s="13"/>
       <c r="E207" s="13"/>
@@ -36864,10 +36878,10 @@
         <v>46000</v>
       </c>
       <c r="B208" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C208" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D208" s="13"/>
       <c r="E208" s="13"/>
@@ -36898,10 +36912,10 @@
         <v>47000</v>
       </c>
       <c r="B209" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C209" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D209" s="13"/>
       <c r="E209" s="13"/>
@@ -36932,10 +36946,10 @@
         <v>50000</v>
       </c>
       <c r="B210" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C210" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D210" s="13"/>
       <c r="E210" s="13"/>
@@ -36966,10 +36980,10 @@
         <v>51000</v>
       </c>
       <c r="B211" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C211" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D211" s="13"/>
       <c r="E211" s="13"/>
@@ -37000,10 +37014,10 @@
         <v>52000</v>
       </c>
       <c r="B212" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C212" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D212" s="13"/>
       <c r="E212" s="13"/>
@@ -37034,10 +37048,10 @@
         <v>53000</v>
       </c>
       <c r="B213" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C213" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D213" s="13"/>
       <c r="E213" s="13"/>
@@ -37068,10 +37082,10 @@
         <v>54000</v>
       </c>
       <c r="B214" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C214" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D214" s="13"/>
       <c r="E214" s="13"/>
@@ -37102,10 +37116,10 @@
         <v>55000</v>
       </c>
       <c r="B215" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C215" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D215" s="13"/>
       <c r="E215" s="13"/>
@@ -37136,10 +37150,10 @@
         <v>56000</v>
       </c>
       <c r="B216" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C216" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D216" s="13"/>
       <c r="E216" s="13"/>
@@ -37170,10 +37184,10 @@
         <v>90000</v>
       </c>
       <c r="B217" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C217" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D217" s="13"/>
       <c r="E217" s="13"/>
@@ -37204,10 +37218,10 @@
         <v>44001</v>
       </c>
       <c r="B218" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C218" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D218" s="13"/>
       <c r="E218" s="13"/>
@@ -37238,10 +37252,10 @@
         <v>44003</v>
       </c>
       <c r="B219" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C219" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D219" s="13"/>
       <c r="E219" s="13"/>
@@ -37272,10 +37286,10 @@
         <v>44002</v>
       </c>
       <c r="B220" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C220" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D220" s="13"/>
       <c r="E220" s="13"/>
@@ -37306,10 +37320,10 @@
         <v>44004</v>
       </c>
       <c r="B221" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C221" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D221" s="13"/>
       <c r="E221" s="13"/>
@@ -37340,10 +37354,10 @@
         <v>47002</v>
       </c>
       <c r="B222" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C222" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D222" s="13"/>
       <c r="E222" s="13"/>
@@ -37374,10 +37388,10 @@
         <v>47001</v>
       </c>
       <c r="B223" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C223" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D223" s="13"/>
       <c r="E223" s="13"/>
@@ -37408,10 +37422,10 @@
         <v>44009</v>
       </c>
       <c r="B224" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C224" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D224" s="13"/>
       <c r="E224" s="13"/>
@@ -37442,10 +37456,10 @@
         <v>44006</v>
       </c>
       <c r="B225" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C225" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D225" s="13"/>
       <c r="E225" s="13"/>
@@ -37476,10 +37490,10 @@
         <v>44008</v>
       </c>
       <c r="B226" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C226" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D226" s="13"/>
       <c r="E226" s="13"/>
@@ -37510,10 +37524,10 @@
         <v>7002</v>
       </c>
       <c r="B227" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C227" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D227" s="13"/>
       <c r="E227" s="13"/>
@@ -37544,10 +37558,10 @@
         <v>7003</v>
       </c>
       <c r="B228" s="13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C228" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D228" s="13"/>
       <c r="E228" s="13"/>
@@ -37578,10 +37592,10 @@
         <v>44012</v>
       </c>
       <c r="B229" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C229" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D229" s="13"/>
       <c r="E229" s="13"/>
@@ -37612,10 +37626,10 @@
         <v>44014</v>
       </c>
       <c r="B230" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C230" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D230" s="13"/>
       <c r="E230" s="13"/>
@@ -37646,10 +37660,10 @@
         <v>44011</v>
       </c>
       <c r="B231" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C231" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D231" s="13"/>
       <c r="E231" s="13"/>
@@ -37680,10 +37694,10 @@
         <v>44015</v>
       </c>
       <c r="B232" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C232" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D232" s="13"/>
       <c r="E232" s="13"/>
@@ -37714,10 +37728,10 @@
         <v>44005</v>
       </c>
       <c r="B233" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C233" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D233" s="13"/>
       <c r="E233" s="13"/>
@@ -37748,10 +37762,10 @@
         <v>43001</v>
       </c>
       <c r="B234" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C234" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D234" s="13"/>
       <c r="E234" s="13"/>
@@ -37782,10 +37796,10 @@
         <v>2004</v>
       </c>
       <c r="B235" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C235" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D235" s="13"/>
       <c r="E235" s="13"/>
@@ -37816,10 +37830,10 @@
         <v>2003</v>
       </c>
       <c r="B236" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C236" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D236" s="13"/>
       <c r="E236" s="13"/>
@@ -37850,10 +37864,10 @@
         <v>2002</v>
       </c>
       <c r="B237" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C237" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D237" s="13"/>
       <c r="E237" s="13"/>
@@ -37884,10 +37898,10 @@
         <v>2005</v>
       </c>
       <c r="B238" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C238" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D238" s="13"/>
       <c r="E238" s="13"/>
@@ -37918,10 +37932,10 @@
         <v>6002</v>
       </c>
       <c r="B239" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C239" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D239" s="13"/>
       <c r="E239" s="13"/>
@@ -37952,10 +37966,10 @@
         <v>6003</v>
       </c>
       <c r="B240" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C240" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D240" s="13"/>
       <c r="E240" s="13"/>
@@ -37986,10 +38000,10 @@
         <v>3</v>
       </c>
       <c r="B241" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C241" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D241" s="13"/>
       <c r="E241" s="13"/>
@@ -38020,10 +38034,10 @@
         <v>4</v>
       </c>
       <c r="B242" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C242" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D242" s="13"/>
       <c r="E242" s="13"/>
@@ -38054,10 +38068,10 @@
         <v>0</v>
       </c>
       <c r="B243" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C243" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D243" s="13"/>
       <c r="E243" s="13"/>
@@ -38088,10 +38102,10 @@
         <v>1</v>
       </c>
       <c r="B244" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C244" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D244" s="13"/>
       <c r="E244" s="13"/>
@@ -38122,10 +38136,10 @@
         <v>252</v>
       </c>
       <c r="B245" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C245" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D245" s="13"/>
       <c r="E245" s="13"/>
@@ -38156,10 +38170,10 @@
         <v>251</v>
       </c>
       <c r="B246" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C246" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D246" s="13"/>
       <c r="E246" s="13"/>
@@ -38190,10 +38204,10 @@
         <v>255</v>
       </c>
       <c r="B247" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C247" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D247" s="13"/>
       <c r="E247" s="13"/>
@@ -38224,10 +38238,10 @@
         <v>250</v>
       </c>
       <c r="B248" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C248" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D248" s="13"/>
       <c r="E248" s="13"/>
@@ -38258,10 +38272,10 @@
         <v>254</v>
       </c>
       <c r="B249" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C249" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D249" s="13"/>
       <c r="E249" s="13"/>
@@ -38292,10 +38306,10 @@
         <v>2</v>
       </c>
       <c r="B250" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C250" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D250" s="13"/>
       <c r="E250" s="13"/>
@@ -38326,10 +38340,10 @@
         <v>253</v>
       </c>
       <c r="B251" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C251" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D251" s="13"/>
       <c r="E251" s="13"/>
@@ -38360,7 +38374,7 @@
         <v>3</v>
       </c>
       <c r="B252" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C252" s="14" t="s">
         <v>22</v>
@@ -38394,7 +38408,7 @@
         <v>4</v>
       </c>
       <c r="B253" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C253" s="14" t="s">
         <v>22</v>
@@ -38428,7 +38442,7 @@
         <v>2</v>
       </c>
       <c r="B254" s="13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C254" s="14" t="s">
         <v>22</v>
@@ -38462,7 +38476,7 @@
         <v>252</v>
       </c>
       <c r="B255" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C255" s="14" t="s">
         <v>22</v>
@@ -38496,7 +38510,7 @@
         <v>255</v>
       </c>
       <c r="B256" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C256" s="14" t="s">
         <v>22</v>
@@ -38530,7 +38544,7 @@
         <v>250</v>
       </c>
       <c r="B257" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C257" s="14" t="s">
         <v>22</v>
@@ -38564,7 +38578,7 @@
         <v>1</v>
       </c>
       <c r="B258" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C258" s="14" t="s">
         <v>22</v>
@@ -38598,10 +38612,10 @@
         <v>8</v>
       </c>
       <c r="B259" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C259" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D259" s="13"/>
       <c r="E259" s="13"/>
@@ -38632,10 +38646,10 @@
         <v>4</v>
       </c>
       <c r="B260" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C260" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D260" s="13"/>
       <c r="E260" s="13"/>
@@ -38666,10 +38680,10 @@
         <v>1</v>
       </c>
       <c r="B261" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C261" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D261" s="13"/>
       <c r="E261" s="13"/>
@@ -38700,10 +38714,10 @@
         <v>2</v>
       </c>
       <c r="B262" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C262" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D262" s="13"/>
       <c r="E262" s="13"/>
@@ -38734,10 +38748,10 @@
         <v>10</v>
       </c>
       <c r="B263" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C263" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D263" s="13"/>
       <c r="E263" s="13"/>
@@ -38768,10 +38782,10 @@
         <v>5</v>
       </c>
       <c r="B264" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C264" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D264" s="13"/>
       <c r="E264" s="13"/>
@@ -38802,10 +38816,10 @@
         <v>6</v>
       </c>
       <c r="B265" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C265" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D265" s="13"/>
       <c r="E265" s="13"/>
@@ -38836,10 +38850,10 @@
         <v>0</v>
       </c>
       <c r="B266" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C266" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D266" s="13"/>
       <c r="E266" s="13"/>
@@ -38870,10 +38884,10 @@
         <v>252</v>
       </c>
       <c r="B267" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C267" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D267" s="13"/>
       <c r="E267" s="13"/>
@@ -38904,10 +38918,10 @@
         <v>251</v>
       </c>
       <c r="B268" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C268" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D268" s="13"/>
       <c r="E268" s="13"/>
@@ -38938,10 +38952,10 @@
         <v>255</v>
       </c>
       <c r="B269" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C269" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D269" s="13"/>
       <c r="E269" s="13"/>
@@ -38972,10 +38986,10 @@
         <v>250</v>
       </c>
       <c r="B270" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C270" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D270" s="13"/>
       <c r="E270" s="13"/>
@@ -39006,10 +39020,10 @@
         <v>11</v>
       </c>
       <c r="B271" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C271" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D271" s="13"/>
       <c r="E271" s="13"/>
@@ -39040,10 +39054,10 @@
         <v>3</v>
       </c>
       <c r="B272" s="13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C272" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D272" s="13"/>
       <c r="E272" s="13"/>
@@ -39074,10 +39088,10 @@
         <v>7</v>
       </c>
       <c r="B273" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C273" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D273" s="13"/>
       <c r="E273" s="13"/>
@@ -39108,10 +39122,10 @@
         <v>9</v>
       </c>
       <c r="B274" s="13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C274" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D274" s="13"/>
       <c r="E274" s="13"/>
@@ -39142,10 +39156,10 @@
         <v>254</v>
       </c>
       <c r="B275" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C275" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D275" s="13"/>
       <c r="E275" s="13"/>
@@ -39176,10 +39190,10 @@
         <v>253</v>
       </c>
       <c r="B276" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C276" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D276" s="13"/>
       <c r="E276" s="13"/>
@@ -39210,10 +39224,10 @@
         <v>7</v>
       </c>
       <c r="B277" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C277" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D277" s="13"/>
       <c r="E277" s="13"/>
@@ -39244,10 +39258,10 @@
         <v>2</v>
       </c>
       <c r="B278" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C278" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D278" s="13"/>
       <c r="E278" s="13"/>
@@ -39278,10 +39292,10 @@
         <v>1</v>
       </c>
       <c r="B279" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C279" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D279" s="13"/>
       <c r="E279" s="13"/>
@@ -39312,10 +39326,10 @@
         <v>3</v>
       </c>
       <c r="B280" s="13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C280" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D280" s="13"/>
       <c r="E280" s="13"/>
@@ -39346,10 +39360,10 @@
         <v>4</v>
       </c>
       <c r="B281" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C281" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D281" s="13"/>
       <c r="E281" s="13"/>
@@ -39380,10 +39394,10 @@
         <v>15</v>
       </c>
       <c r="B282" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C282" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D282" s="13"/>
       <c r="E282" s="13"/>
@@ -39414,10 +39428,10 @@
         <v>6</v>
       </c>
       <c r="B283" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C283" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D283" s="13"/>
       <c r="E283" s="13"/>
@@ -39448,10 +39462,10 @@
         <v>16</v>
       </c>
       <c r="B284" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C284" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D284" s="13"/>
       <c r="E284" s="13"/>
@@ -39482,10 +39496,10 @@
         <v>5</v>
       </c>
       <c r="B285" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C285" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D285" s="13"/>
       <c r="E285" s="13"/>
@@ -39516,10 +39530,10 @@
         <v>13</v>
       </c>
       <c r="B286" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C286" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D286" s="13"/>
       <c r="E286" s="13"/>
@@ -39550,10 +39564,10 @@
         <v>252</v>
       </c>
       <c r="B287" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C287" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D287" s="13"/>
       <c r="E287" s="13"/>
@@ -39584,10 +39598,10 @@
         <v>251</v>
       </c>
       <c r="B288" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C288" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D288" s="13"/>
       <c r="E288" s="13"/>
@@ -39618,10 +39632,10 @@
         <v>255</v>
       </c>
       <c r="B289" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C289" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D289" s="13"/>
       <c r="E289" s="13"/>
@@ -39652,10 +39666,10 @@
         <v>9</v>
       </c>
       <c r="B290" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C290" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D290" s="13"/>
       <c r="E290" s="13"/>
@@ -39686,10 +39700,10 @@
         <v>250</v>
       </c>
       <c r="B291" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C291" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D291" s="13"/>
       <c r="E291" s="13"/>
@@ -39720,10 +39734,10 @@
         <v>10</v>
       </c>
       <c r="B292" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C292" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D292" s="13"/>
       <c r="E292" s="13"/>
@@ -39754,10 +39768,10 @@
         <v>11</v>
       </c>
       <c r="B293" s="13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C293" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D293" s="13"/>
       <c r="E293" s="13"/>
@@ -39788,10 +39802,10 @@
         <v>14</v>
       </c>
       <c r="B294" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C294" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D294" s="13"/>
       <c r="E294" s="13"/>
@@ -39822,10 +39836,10 @@
         <v>254</v>
       </c>
       <c r="B295" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C295" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D295" s="13"/>
       <c r="E295" s="13"/>
@@ -39856,10 +39870,10 @@
         <v>253</v>
       </c>
       <c r="B296" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C296" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D296" s="13"/>
       <c r="E296" s="13"/>
@@ -39890,10 +39904,10 @@
         <v>8</v>
       </c>
       <c r="B297" s="13" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C297" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D297" s="13"/>
       <c r="E297" s="13"/>
@@ -39924,10 +39938,10 @@
         <v>12</v>
       </c>
       <c r="B298" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C298" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D298" s="13"/>
       <c r="E298" s="13"/>
@@ -39958,10 +39972,10 @@
         <v>1</v>
       </c>
       <c r="B299" s="13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C299" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D299" s="13"/>
       <c r="E299" s="13"/>
@@ -39992,10 +40006,10 @@
         <v>6</v>
       </c>
       <c r="B300" s="13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C300" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D300" s="13"/>
       <c r="E300" s="13"/>
@@ -40026,10 +40040,10 @@
         <v>5</v>
       </c>
       <c r="B301" s="13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C301" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D301" s="13"/>
       <c r="E301" s="13"/>
@@ -40060,10 +40074,10 @@
         <v>4</v>
       </c>
       <c r="B302" s="13" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C302" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D302" s="13"/>
       <c r="E302" s="13"/>
@@ -40094,10 +40108,10 @@
         <v>3</v>
       </c>
       <c r="B303" s="13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C303" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D303" s="13"/>
       <c r="E303" s="13"/>
@@ -40128,10 +40142,10 @@
         <v>2</v>
       </c>
       <c r="B304" s="13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C304" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D304" s="13"/>
       <c r="E304" s="13"/>
@@ -40162,10 +40176,10 @@
         <v>23</v>
       </c>
       <c r="B305" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C305" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D305" s="13"/>
       <c r="E305" s="13"/>
@@ -40196,10 +40210,10 @@
         <v>24</v>
       </c>
       <c r="B306" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C306" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D306" s="13"/>
       <c r="E306" s="13"/>
@@ -40230,10 +40244,10 @@
         <v>25</v>
       </c>
       <c r="B307" s="13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C307" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D307" s="13"/>
       <c r="E307" s="13"/>
@@ -40264,10 +40278,10 @@
         <v>14</v>
       </c>
       <c r="B308" s="13" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C308" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D308" s="13"/>
       <c r="E308" s="13"/>
@@ -40298,10 +40312,10 @@
         <v>26</v>
       </c>
       <c r="B309" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C309" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D309" s="13"/>
       <c r="E309" s="13"/>
@@ -40332,10 +40346,10 @@
         <v>22</v>
       </c>
       <c r="B310" s="13" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C310" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D310" s="13"/>
       <c r="E310" s="13"/>
@@ -40366,10 +40380,10 @@
         <v>15</v>
       </c>
       <c r="B311" s="13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C311" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D311" s="13"/>
       <c r="E311" s="13"/>
@@ -40400,10 +40414,10 @@
         <v>17</v>
       </c>
       <c r="B312" s="13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C312" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D312" s="13"/>
       <c r="E312" s="13"/>
@@ -40434,10 +40448,10 @@
         <v>16</v>
       </c>
       <c r="B313" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C313" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D313" s="13"/>
       <c r="E313" s="13"/>
@@ -40468,10 +40482,10 @@
         <v>13</v>
       </c>
       <c r="B314" s="13" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C314" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D314" s="13"/>
       <c r="E314" s="13"/>
@@ -40502,10 +40516,10 @@
         <v>252</v>
       </c>
       <c r="B315" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C315" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D315" s="13"/>
       <c r="E315" s="13"/>
@@ -40536,10 +40550,10 @@
         <v>251</v>
       </c>
       <c r="B316" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C316" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D316" s="13"/>
       <c r="E316" s="13"/>
@@ -40570,10 +40584,10 @@
         <v>255</v>
       </c>
       <c r="B317" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C317" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D317" s="13"/>
       <c r="E317" s="13"/>
@@ -40604,10 +40618,10 @@
         <v>250</v>
       </c>
       <c r="B318" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C318" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D318" s="13"/>
       <c r="E318" s="13"/>
@@ -40638,10 +40652,10 @@
         <v>10</v>
       </c>
       <c r="B319" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C319" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D319" s="13"/>
       <c r="E319" s="13"/>
@@ -40672,10 +40686,10 @@
         <v>11</v>
       </c>
       <c r="B320" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C320" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D320" s="13"/>
       <c r="E320" s="13"/>
@@ -40706,10 +40720,10 @@
         <v>12</v>
       </c>
       <c r="B321" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C321" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D321" s="13"/>
       <c r="E321" s="13"/>
@@ -40740,10 +40754,10 @@
         <v>7</v>
       </c>
       <c r="B322" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C322" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D322" s="13"/>
       <c r="E322" s="13"/>
@@ -40774,10 +40788,10 @@
         <v>8</v>
       </c>
       <c r="B323" s="13" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C323" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D323" s="13"/>
       <c r="E323" s="13"/>
@@ -40808,10 +40822,10 @@
         <v>9</v>
       </c>
       <c r="B324" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C324" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D324" s="13"/>
       <c r="E324" s="13"/>
@@ -40842,10 +40856,10 @@
         <v>18</v>
       </c>
       <c r="B325" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C325" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D325" s="13"/>
       <c r="E325" s="13"/>
@@ -40876,10 +40890,10 @@
         <v>20</v>
       </c>
       <c r="B326" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C326" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D326" s="13"/>
       <c r="E326" s="13"/>
@@ -40910,10 +40924,10 @@
         <v>19</v>
       </c>
       <c r="B327" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C327" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D327" s="13"/>
       <c r="E327" s="13"/>
@@ -40944,10 +40958,10 @@
         <v>254</v>
       </c>
       <c r="B328" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C328" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D328" s="13"/>
       <c r="E328" s="13"/>
@@ -40978,10 +40992,10 @@
         <v>253</v>
       </c>
       <c r="B329" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C329" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D329" s="13"/>
       <c r="E329" s="13"/>
@@ -41012,10 +41026,10 @@
         <v>21</v>
       </c>
       <c r="B330" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C330" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D330" s="13"/>
       <c r="E330" s="13"/>
@@ -41046,10 +41060,10 @@
         <v>1</v>
       </c>
       <c r="B331" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C331" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D331" s="13"/>
       <c r="E331" s="13"/>
@@ -41080,10 +41094,10 @@
         <v>2</v>
       </c>
       <c r="B332" s="16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C332" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D332" s="13"/>
       <c r="E332" s="13"/>
@@ -41114,10 +41128,10 @@
         <v>251</v>
       </c>
       <c r="B333" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C333" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D333" s="13"/>
       <c r="E333" s="13"/>

</xml_diff>